<commit_message>
updated data to include broadband dept
</commit_message>
<xml_diff>
--- a/public/budget_data_2014.xlsx
+++ b/public/budget_data_2014.xlsx
@@ -16,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Raw data'!$A$1:$A$699</definedName>
     <definedName name="_xlnm.Extract" localSheetId="1">'Raw data'!$A$705</definedName>
   </definedNames>
-  <calcPr calcId="140001" calcMode="autoNoTable" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:CRTarget Flags="-1"/>
@@ -335,7 +335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8198" uniqueCount="1002">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8366" uniqueCount="1025">
   <si>
     <t>Defence portfolio</t>
   </si>
@@ -3341,6 +3341,75 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Broadband and Communications Infrastructure</t>
+  </si>
+  <si>
+    <t>Digital Economy and Postal Services</t>
+  </si>
+  <si>
+    <t>Broadcasting and Digital Television</t>
+  </si>
+  <si>
+    <t>Department of Broadband, Communications and the Digital Economy</t>
+  </si>
+  <si>
+    <t>Australian Broadcasting Corporation</t>
+  </si>
+  <si>
+    <t>ABC Radio</t>
+  </si>
+  <si>
+    <t>ABC Television</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>ABC Analog Transmission</t>
+  </si>
+  <si>
+    <t>Access to digital TV services</t>
+  </si>
+  <si>
+    <t>Access to digital radio services</t>
+  </si>
+  <si>
+    <t>Australian Communications and Media Authority</t>
+  </si>
+  <si>
+    <t>Communications regulation, planning and licensing</t>
+  </si>
+  <si>
+    <t>Consumer safeguards, education and information</t>
+  </si>
+  <si>
+    <t>Special Broadcasting Service Corporation</t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Analog Transmission and Distribution</t>
+  </si>
+  <si>
+    <t>Digital TV Transmission and Distribution</t>
+  </si>
+  <si>
+    <t>Digital Radio Transmission and Distribution</t>
+  </si>
+  <si>
+    <t>Telecommunications Universal Service Management Agency</t>
+  </si>
+  <si>
+    <t>http://www.dbcde.gov.au/__data/assets/pdf_file/0004/163417/COMPLETE_BCDE_PBS.pdf</t>
+  </si>
+  <si>
+    <t>Broadband, Communications and the Digital Economy Portfolio Budget Statement</t>
   </si>
 </sst>
 </file>
@@ -3349,7 +3418,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -3439,7 +3508,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1010">
+  <cellStyleXfs count="1032">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4343,6 +4412,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4466,11 +4557,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="902" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="902" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1010">
+  <cellStyles count="1032">
     <cellStyle name="Comma" xfId="902" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -5037,6 +5128,28 @@
     <cellStyle name="Followed Hyperlink" xfId="1007" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1008" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1009" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1010" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1011" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1012" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1013" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1014" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1015" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1016" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1017" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1018" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1019" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1020" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1021" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1022" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1023" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1024" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1025" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1026" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1027" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1028" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1029" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1030" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1031" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6006,7 +6119,7 @@
       </c>
       <c r="C22" s="8">
         <f>SUMIF('Raw data'!$A$2:$A$1008,B22,'Raw data'!$G$2:$G$1008)/1000</f>
-        <v>0</v>
+        <v>2388.6640000000002</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -6015,7 +6128,7 @@
       </c>
       <c r="C23" s="10">
         <f>SUM(C3:C22)</f>
-        <v>424062.11199999991</v>
+        <v>426450.7759999999</v>
       </c>
     </row>
   </sheetData>
@@ -6023,7 +6136,6 @@
     <sortCondition descending="1" ref="C3:C22"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6036,8 +6148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1068"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L753"/>
+    <sheetView topLeftCell="A749" workbookViewId="0">
+      <selection activeCell="A770" sqref="A1:L770"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -27754,186 +27866,506 @@
       </c>
     </row>
     <row r="754" spans="1:12">
-      <c r="F754" s="1"/>
-      <c r="G754" s="1"/>
+      <c r="A754" t="s">
+        <v>992</v>
+      </c>
+      <c r="B754" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C754" t="s">
+        <v>1002</v>
+      </c>
+      <c r="F754" s="1">
+        <v>70710</v>
+      </c>
+      <c r="G754" s="1">
+        <v>48519</v>
+      </c>
       <c r="H754" s="1"/>
       <c r="I754" s="1"/>
+      <c r="K754" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L754" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="755" spans="1:12">
-      <c r="F755" s="1"/>
-      <c r="G755" s="1"/>
+      <c r="A755" t="s">
+        <v>992</v>
+      </c>
+      <c r="B755" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C755" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F755" s="1">
+        <v>98301</v>
+      </c>
+      <c r="G755" s="1">
+        <v>95983</v>
+      </c>
       <c r="H755" s="1"/>
       <c r="I755" s="1"/>
+      <c r="K755" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L755" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="756" spans="1:12">
-      <c r="F756" s="1"/>
-      <c r="G756" s="1"/>
+      <c r="A756" t="s">
+        <v>992</v>
+      </c>
+      <c r="B756" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C756" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F756" s="1">
+        <v>268066</v>
+      </c>
+      <c r="G756" s="1">
+        <v>210896</v>
+      </c>
       <c r="H756" s="1"/>
       <c r="I756" s="1"/>
+      <c r="K756" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L756" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="757" spans="1:12">
-      <c r="F757" s="1"/>
-      <c r="G757" s="1"/>
+      <c r="A757" t="s">
+        <v>992</v>
+      </c>
+      <c r="B757" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C757" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F757" s="1">
+        <v>337691</v>
+      </c>
+      <c r="G757" s="1">
+        <v>348571</v>
+      </c>
       <c r="H757" s="1"/>
       <c r="I757" s="1"/>
+      <c r="K757" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L757" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="758" spans="1:12">
-      <c r="F758" s="1"/>
-      <c r="G758" s="1"/>
+      <c r="A758" t="s">
+        <v>992</v>
+      </c>
+      <c r="B758" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C758" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F758" s="1">
+        <v>627150</v>
+      </c>
+      <c r="G758" s="1">
+        <v>647348</v>
+      </c>
       <c r="H758" s="1"/>
       <c r="I758" s="1"/>
+      <c r="K758" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L758" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="759" spans="1:12">
-      <c r="F759" s="1"/>
-      <c r="G759" s="1"/>
+      <c r="A759" t="s">
+        <v>992</v>
+      </c>
+      <c r="B759" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C759" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F759" s="1">
+        <v>25755</v>
+      </c>
+      <c r="G759" s="1">
+        <v>26587</v>
+      </c>
       <c r="H759" s="1"/>
       <c r="I759" s="1"/>
+      <c r="K759" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L759" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="760" spans="1:12">
-      <c r="F760" s="1"/>
-      <c r="G760" s="1"/>
+      <c r="A760" t="s">
+        <v>992</v>
+      </c>
+      <c r="B760" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C760" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F760" s="1">
+        <v>88669</v>
+      </c>
+      <c r="G760" s="1">
+        <v>80403</v>
+      </c>
       <c r="H760" s="1"/>
       <c r="I760" s="1"/>
+      <c r="K760" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L760" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="761" spans="1:12">
-      <c r="F761" s="1"/>
-      <c r="G761" s="1"/>
+      <c r="A761" t="s">
+        <v>992</v>
+      </c>
+      <c r="B761" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C761" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F761" s="1">
+        <v>100673</v>
+      </c>
+      <c r="G761" s="1">
+        <v>109103</v>
+      </c>
       <c r="H761" s="1"/>
       <c r="I761" s="1"/>
+      <c r="K761" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L761" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="762" spans="1:12">
-      <c r="F762" s="1"/>
-      <c r="G762" s="1"/>
+      <c r="A762" t="s">
+        <v>992</v>
+      </c>
+      <c r="B762" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C762" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F762" s="1">
+        <v>3658</v>
+      </c>
+      <c r="G762" s="1">
+        <v>3705</v>
+      </c>
       <c r="H762" s="1"/>
       <c r="I762" s="1"/>
+      <c r="K762" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L762" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="763" spans="1:12">
-      <c r="F763" s="1"/>
-      <c r="G763" s="1"/>
+      <c r="A763" t="s">
+        <v>992</v>
+      </c>
+      <c r="B763" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C763" t="s">
+        <v>1014</v>
+      </c>
+      <c r="F763" s="1">
+        <v>73430</v>
+      </c>
+      <c r="G763" s="1">
+        <v>68150</v>
+      </c>
       <c r="H763" s="1"/>
       <c r="I763" s="1"/>
+      <c r="K763" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L763" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="764" spans="1:12">
-      <c r="F764" s="1"/>
-      <c r="G764" s="1"/>
+      <c r="A764" t="s">
+        <v>992</v>
+      </c>
+      <c r="B764" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C764" t="s">
+        <v>1015</v>
+      </c>
+      <c r="F764" s="1">
+        <v>86052</v>
+      </c>
+      <c r="G764" s="1">
+        <v>25487</v>
+      </c>
       <c r="H764" s="1"/>
       <c r="I764" s="1"/>
+      <c r="K764" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L764" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="765" spans="1:12">
-      <c r="F765" s="1"/>
-      <c r="G765" s="1"/>
+      <c r="A765" t="s">
+        <v>992</v>
+      </c>
+      <c r="B765" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C765" t="s">
+        <v>1017</v>
+      </c>
+      <c r="F765" s="1">
+        <v>214488</v>
+      </c>
+      <c r="G765" s="1">
+        <v>250057</v>
+      </c>
       <c r="H765" s="1"/>
       <c r="I765" s="1"/>
+      <c r="K765" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L765" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="766" spans="1:12">
-      <c r="F766" s="1"/>
-      <c r="G766" s="1"/>
+      <c r="A766" t="s">
+        <v>992</v>
+      </c>
+      <c r="B766" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C766" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F766" s="1">
+        <v>37518</v>
+      </c>
+      <c r="G766" s="1">
+        <v>40474</v>
+      </c>
       <c r="H766" s="1"/>
       <c r="I766" s="1"/>
+      <c r="K766" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L766" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="767" spans="1:12">
-      <c r="F767" s="1"/>
-      <c r="G767" s="1"/>
+      <c r="A767" t="s">
+        <v>992</v>
+      </c>
+      <c r="B767" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C767" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F767" s="1">
+        <v>11017</v>
+      </c>
+      <c r="G767" s="1">
+        <v>3420</v>
+      </c>
       <c r="H767" s="1"/>
       <c r="I767" s="1"/>
+      <c r="K767" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L767" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="768" spans="1:12">
-      <c r="F768" s="1"/>
-      <c r="G768" s="1"/>
+      <c r="A768" t="s">
+        <v>992</v>
+      </c>
+      <c r="B768" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C768" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F768" s="1">
+        <v>69069</v>
+      </c>
+      <c r="G768" s="1">
+        <v>81440</v>
+      </c>
       <c r="H768" s="1"/>
       <c r="I768" s="1"/>
-    </row>
-    <row r="769" spans="6:9">
-      <c r="F769" s="1"/>
-      <c r="G769" s="1"/>
+      <c r="K768" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L768" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="769" spans="1:12">
+      <c r="A769" t="s">
+        <v>992</v>
+      </c>
+      <c r="B769" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C769" t="s">
+        <v>1021</v>
+      </c>
+      <c r="F769" s="1">
+        <v>2030</v>
+      </c>
+      <c r="G769" s="1">
+        <v>2064</v>
+      </c>
       <c r="H769" s="1"/>
       <c r="I769" s="1"/>
-    </row>
-    <row r="770" spans="6:9">
-      <c r="F770" s="1"/>
-      <c r="G770" s="1"/>
+      <c r="K769" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L769" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="770" spans="1:12">
+      <c r="A770" t="s">
+        <v>992</v>
+      </c>
+      <c r="B770" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F770" s="1">
+        <v>313565</v>
+      </c>
+      <c r="G770" s="1">
+        <v>346457</v>
+      </c>
       <c r="H770" s="1"/>
       <c r="I770" s="1"/>
-    </row>
-    <row r="771" spans="6:9">
+      <c r="K770" t="s">
+        <v>1024</v>
+      </c>
+      <c r="L770" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="771" spans="1:12">
       <c r="F771" s="1"/>
       <c r="G771" s="1"/>
       <c r="H771" s="1"/>
       <c r="I771" s="1"/>
     </row>
-    <row r="772" spans="6:9">
+    <row r="772" spans="1:12">
       <c r="F772" s="1"/>
       <c r="G772" s="1"/>
       <c r="H772" s="1"/>
       <c r="I772" s="1"/>
     </row>
-    <row r="773" spans="6:9">
+    <row r="773" spans="1:12">
       <c r="F773" s="1"/>
       <c r="G773" s="1"/>
       <c r="H773" s="1"/>
       <c r="I773" s="1"/>
     </row>
-    <row r="774" spans="6:9">
+    <row r="774" spans="1:12">
       <c r="F774" s="1"/>
       <c r="G774" s="1"/>
       <c r="H774" s="1"/>
       <c r="I774" s="1"/>
     </row>
-    <row r="775" spans="6:9">
+    <row r="775" spans="1:12">
       <c r="F775" s="1"/>
       <c r="G775" s="1"/>
       <c r="H775" s="1"/>
       <c r="I775" s="1"/>
     </row>
-    <row r="776" spans="6:9">
+    <row r="776" spans="1:12">
       <c r="F776" s="1"/>
       <c r="G776" s="1"/>
       <c r="H776" s="1"/>
       <c r="I776" s="1"/>
     </row>
-    <row r="777" spans="6:9">
+    <row r="777" spans="1:12">
       <c r="F777" s="1"/>
       <c r="G777" s="1"/>
       <c r="H777" s="1"/>
       <c r="I777" s="1"/>
     </row>
-    <row r="778" spans="6:9">
+    <row r="778" spans="1:12">
       <c r="F778" s="1"/>
       <c r="G778" s="1"/>
       <c r="H778" s="1"/>
       <c r="I778" s="1"/>
     </row>
-    <row r="779" spans="6:9">
+    <row r="779" spans="1:12">
       <c r="F779" s="1"/>
       <c r="G779" s="1"/>
       <c r="H779" s="1"/>
       <c r="I779" s="1"/>
     </row>
-    <row r="780" spans="6:9">
+    <row r="780" spans="1:12">
       <c r="F780" s="1"/>
       <c r="G780" s="1"/>
       <c r="H780" s="1"/>
       <c r="I780" s="1"/>
     </row>
-    <row r="781" spans="6:9">
+    <row r="781" spans="1:12">
       <c r="F781" s="1"/>
       <c r="G781" s="1"/>
       <c r="H781" s="1"/>
       <c r="I781" s="1"/>
     </row>
-    <row r="782" spans="6:9">
+    <row r="782" spans="1:12">
       <c r="F782" s="1"/>
       <c r="G782" s="1"/>
       <c r="H782" s="1"/>
       <c r="I782" s="1"/>
     </row>
-    <row r="783" spans="6:9">
+    <row r="783" spans="1:12">
       <c r="F783" s="1"/>
       <c r="G783" s="1"/>
       <c r="H783" s="1"/>
       <c r="I783" s="1"/>
     </row>
-    <row r="784" spans="6:9">
+    <row r="784" spans="1:12">
       <c r="F784" s="1"/>
       <c r="G784" s="1"/>
       <c r="H784" s="1"/>
@@ -29802,10 +30234,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J753"/>
+  <dimension ref="A1:J770"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A561" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A677" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -29832,7 +30264,7 @@
       <c r="G1" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>101</v>
       </c>
       <c r="I1" t="s">
@@ -48168,6 +48600,394 @@
       </c>
       <c r="J753" t="s">
         <v>990</v>
+      </c>
+    </row>
+    <row r="754" spans="1:10">
+      <c r="A754" t="s">
+        <v>992</v>
+      </c>
+      <c r="B754" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C754" t="s">
+        <v>1002</v>
+      </c>
+      <c r="F754">
+        <v>70710</v>
+      </c>
+      <c r="G754">
+        <v>48519</v>
+      </c>
+      <c r="I754" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J754" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="755" spans="1:10">
+      <c r="A755" t="s">
+        <v>992</v>
+      </c>
+      <c r="B755" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C755" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F755">
+        <v>98301</v>
+      </c>
+      <c r="G755">
+        <v>95983</v>
+      </c>
+      <c r="I755" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J755" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="756" spans="1:10">
+      <c r="A756" t="s">
+        <v>992</v>
+      </c>
+      <c r="B756" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C756" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F756">
+        <v>268066</v>
+      </c>
+      <c r="G756">
+        <v>210896</v>
+      </c>
+      <c r="I756" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J756" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="757" spans="1:10">
+      <c r="A757" t="s">
+        <v>992</v>
+      </c>
+      <c r="B757" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C757" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F757">
+        <v>337691</v>
+      </c>
+      <c r="G757">
+        <v>348571</v>
+      </c>
+      <c r="I757" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J757" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="758" spans="1:10">
+      <c r="A758" t="s">
+        <v>992</v>
+      </c>
+      <c r="B758" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C758" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F758">
+        <v>627150</v>
+      </c>
+      <c r="G758">
+        <v>647348</v>
+      </c>
+      <c r="I758" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J758" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="759" spans="1:10">
+      <c r="A759" t="s">
+        <v>992</v>
+      </c>
+      <c r="B759" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C759" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F759">
+        <v>25755</v>
+      </c>
+      <c r="G759">
+        <v>26587</v>
+      </c>
+      <c r="I759" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J759" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="760" spans="1:10">
+      <c r="A760" t="s">
+        <v>992</v>
+      </c>
+      <c r="B760" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C760" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F760">
+        <v>88669</v>
+      </c>
+      <c r="G760">
+        <v>80403</v>
+      </c>
+      <c r="I760" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J760" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="761" spans="1:10">
+      <c r="A761" t="s">
+        <v>992</v>
+      </c>
+      <c r="B761" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C761" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F761">
+        <v>100673</v>
+      </c>
+      <c r="G761">
+        <v>109103</v>
+      </c>
+      <c r="I761" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J761" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="762" spans="1:10">
+      <c r="A762" t="s">
+        <v>992</v>
+      </c>
+      <c r="B762" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C762" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F762">
+        <v>3658</v>
+      </c>
+      <c r="G762">
+        <v>3705</v>
+      </c>
+      <c r="I762" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J762" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="763" spans="1:10">
+      <c r="A763" t="s">
+        <v>992</v>
+      </c>
+      <c r="B763" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C763" t="s">
+        <v>1014</v>
+      </c>
+      <c r="F763">
+        <v>73430</v>
+      </c>
+      <c r="G763">
+        <v>68150</v>
+      </c>
+      <c r="I763" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J763" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="764" spans="1:10">
+      <c r="A764" t="s">
+        <v>992</v>
+      </c>
+      <c r="B764" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C764" t="s">
+        <v>1015</v>
+      </c>
+      <c r="F764">
+        <v>86052</v>
+      </c>
+      <c r="G764">
+        <v>25487</v>
+      </c>
+      <c r="I764" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J764" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="765" spans="1:10">
+      <c r="A765" t="s">
+        <v>992</v>
+      </c>
+      <c r="B765" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C765" t="s">
+        <v>1017</v>
+      </c>
+      <c r="F765">
+        <v>214488</v>
+      </c>
+      <c r="G765">
+        <v>250057</v>
+      </c>
+      <c r="I765" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J765" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="766" spans="1:10">
+      <c r="A766" t="s">
+        <v>992</v>
+      </c>
+      <c r="B766" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C766" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F766">
+        <v>37518</v>
+      </c>
+      <c r="G766">
+        <v>40474</v>
+      </c>
+      <c r="I766" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J766" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="767" spans="1:10">
+      <c r="A767" t="s">
+        <v>992</v>
+      </c>
+      <c r="B767" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C767" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F767">
+        <v>11017</v>
+      </c>
+      <c r="G767">
+        <v>3420</v>
+      </c>
+      <c r="I767" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J767" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="768" spans="1:10">
+      <c r="A768" t="s">
+        <v>992</v>
+      </c>
+      <c r="B768" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C768" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F768">
+        <v>69069</v>
+      </c>
+      <c r="G768">
+        <v>81440</v>
+      </c>
+      <c r="I768" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J768" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="769" spans="1:10">
+      <c r="A769" t="s">
+        <v>992</v>
+      </c>
+      <c r="B769" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C769" t="s">
+        <v>1021</v>
+      </c>
+      <c r="F769">
+        <v>2030</v>
+      </c>
+      <c r="G769">
+        <v>2064</v>
+      </c>
+      <c r="I769" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J769" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="770" spans="1:10">
+      <c r="A770" t="s">
+        <v>992</v>
+      </c>
+      <c r="B770" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F770">
+        <v>313565</v>
+      </c>
+      <c r="G770">
+        <v>346457</v>
+      </c>
+      <c r="I770" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J770" t="s">
+        <v>1023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>